<commit_message>
1. Make VerifyActions Method is Parameterized 2. Other Actions like Dropdown, Radiobuttons, Checkbox, shoule be implemented in actions class. 3. Implement dataprovider in other Modules and Develop with Hashmap 4. Add TestData Description column in Testdata file.
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/Negative Datas.xlsx
+++ b/src/main/resources/Datas/Negative Datas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t xml:space="preserve">Username </t>
   </si>
@@ -995,13 +995,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
@@ -1039,21 +1039,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1063,7 +1053,6 @@
     <hyperlink ref="B3" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
     <hyperlink ref="B4" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
     <hyperlink ref="B5" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
-    <hyperlink ref="B7" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Single method implemented for Edit and Delete actions.
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/Negative Datas.xlsx
+++ b/src/main/resources/Datas/Negative Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7695"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>Test Description</t>
+  </si>
   <si>
     <t xml:space="preserve">Username </t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Correct Username &amp; Wrong Password</t>
   </si>
   <si>
     <t>Vendoadmin</t>
@@ -36,10 +42,19 @@
     <t>Vendo@2023</t>
   </si>
   <si>
+    <t>Wrong Username &amp; Correct Password</t>
+  </si>
+  <si>
     <t>Vendoadmii</t>
   </si>
   <si>
     <t>Vendo@2022</t>
+  </si>
+  <si>
+    <t>Wrong Username &amp; Wrong Password</t>
+  </si>
+  <si>
+    <t>Correct Username &amp; Correct Password</t>
   </si>
 </sst>
 </file>
@@ -48,8 +63,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -73,6 +88,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,15 +125,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -103,6 +180,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -110,110 +225,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -232,91 +247,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,13 +409,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,73 +421,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,6 +438,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -437,11 +467,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -465,51 +516,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -523,151 +529,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -995,64 +1010,80 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="37.3142857142857" customWidth="1"/>
+    <col min="2" max="2" width="13.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="13.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
-    <hyperlink ref="B3" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
-    <hyperlink ref="B4" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
-    <hyperlink ref="B5" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="C2" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
+    <hyperlink ref="C3" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="C4" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
+    <hyperlink ref="C5" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1. Implement dataprovider in other Modules and Develop with Hashmap 2. Add TestData Description column in Testdata file.
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/Negative Datas.xlsx
+++ b/src/main/resources/Datas/Negative Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695"/>
+    <workbookView windowWidth="19815" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>Test Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t xml:space="preserve">Username </t>
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>Correct Username &amp; Wrong Password</t>
   </si>
   <si>
     <t>Vendoadmin</t>
@@ -42,20 +36,11 @@
     <t>Vendo@2023</t>
   </si>
   <si>
-    <t>Wrong Username &amp; Correct Password</t>
-  </si>
-  <si>
     <t>Vendoadmii</t>
   </si>
   <si>
     <t>Vendo@2022</t>
   </si>
-  <si>
-    <t>Wrong Username &amp; Wrong Password</t>
-  </si>
-  <si>
-    <t>Correct Username &amp; Correct Password</t>
-  </si>
 </sst>
 </file>
 
@@ -63,9 +48,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -88,16 +73,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -105,37 +90,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,14 +104,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -165,8 +111,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,9 +182,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,22 +197,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,43 +232,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,139 +412,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,6 +423,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -456,13 +450,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,26 +480,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,157 +515,159 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1010,80 +995,64 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.3142857142857" customWidth="1"/>
-    <col min="2" max="2" width="13.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="13.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>6</v>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>9</v>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
-    <hyperlink ref="C3" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
-    <hyperlink ref="C4" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
-    <hyperlink ref="C5" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="B2" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
+    <hyperlink ref="B3" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="B4" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
+    <hyperlink ref="B5" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1096,7 +1065,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
1. Implement dataprovider in other Modules and Develop with Hashmap 2. Add TestData Description column in Testdata filData driven cases and Asserts are over.
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/Negative Datas.xlsx
+++ b/src/main/resources/Datas/Negative Datas.xlsx
@@ -24,10 +24,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Username </t>
+    <t>USERNAME</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>PASSWORD</t>
   </si>
   <si>
     <t>Vendoadmin</t>
@@ -47,8 +47,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -73,8 +73,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -82,14 +119,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -103,115 +187,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,187 +232,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,8 +429,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -450,50 +450,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,159 +478,196 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -995,13 +995,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
@@ -1046,6 +1046,42 @@
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
30/05/2023 - 1. Logs Completed. 2. Upload Functionality Partially Completed. 3. Browser Value is Added in Extent Report. 4.Common Objects Class is Implemented.
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/Negative Datas.xlsx
+++ b/src/main/resources/Datas/Negative Datas.xlsx
@@ -33,13 +33,13 @@
     <t>Vendoadmin</t>
   </si>
   <si>
-    <t>Vendo@2023</t>
-  </si>
-  <si>
     <t>Vendoadmii</t>
   </si>
   <si>
     <t>Vendo@2022</t>
+  </si>
+  <si>
+    <t>Vendo@2023</t>
   </si>
 </sst>
 </file>
@@ -47,10 +47,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -74,62 +74,55 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,8 +134,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -157,46 +158,52 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,14 +211,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,13 +232,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,169 +412,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,42 +435,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -500,21 +474,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -523,151 +482,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -998,7 +998,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E7" sqref="A2 G11 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1019,24 +1019,24 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1085,10 +1085,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
-    <hyperlink ref="B3" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
-    <hyperlink ref="B4" r:id="rId1" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
-    <hyperlink ref="B5" r:id="rId2" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="B5" r:id="rId1" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="B3" r:id="rId1" display="Vendo@2022" tooltip="mailto:Vendo@2022"/>
+    <hyperlink ref="B4" r:id="rId2" display="Vendo@2023" tooltip="mailto:Vendo@2023"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>